<commit_message>
repo update and project card title font
</commit_message>
<xml_diff>
--- a/projects/CADS-covid-topic-modeling/CADS_metadata.xlsx
+++ b/projects/CADS-covid-topic-modeling/CADS_metadata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tvedt/Documents/GitHub/sva-codelib/projects/siri1/CADS-covid-topic-modelling/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tvedt/Documents/GitHub/sva-codelib/projects/CADS-covid-topic-modeling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2834DAC8-CDB5-6948-A8DD-FADFBF53D4D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A5C7EE1-C5C5-2842-8513-C02353B4B89F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4300" yWindow="2800" windowWidth="21600" windowHeight="11300" xr2:uid="{E69FBF4E-0996-4780-9349-3F26039E9820}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>title</t>
   </si>
@@ -62,9 +62,6 @@
     <t>themes</t>
   </si>
   <si>
-    <t>Sosiale medier, tekstanalyse, misinformasjon</t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
@@ -74,10 +71,25 @@
     <t>Undersøker diskursive trender innen vaksinemisinformasjon fra COVID-19 pandemien. Les mer her: https://doi.org/10.1177/20563051251347614</t>
   </si>
   <si>
-    <t>Topic modeling, sentiment analysis, mixed-methods</t>
-  </si>
-  <si>
     <t>text corpus</t>
+  </si>
+  <si>
+    <t>sentiment analysis</t>
+  </si>
+  <si>
+    <t>mixed-methods</t>
+  </si>
+  <si>
+    <t>Topic modeling</t>
+  </si>
+  <si>
+    <t>misinformasjon</t>
+  </si>
+  <si>
+    <t>tekstanalyse</t>
+  </si>
+  <si>
+    <t>Sosiale medier</t>
   </si>
 </sst>
 </file>
@@ -449,23 +461,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E34B38C-8714-4516-B8FD-2AA6BB15744E}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="8.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -473,7 +488,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -481,36 +496,48 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>